<commit_message>
The end part2 :p
</commit_message>
<xml_diff>
--- a/public/helloworld.xlsx
+++ b/public/helloworld.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -26,22 +26,28 @@
     <t>Tournoi</t>
   </si>
   <si>
+    <t>samis</t>
+  </si>
+  <si>
+    <t>platinum</t>
+  </si>
+  <si>
+    <t>sgs</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>bronze</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
     <t>sami</t>
   </si>
   <si>
-    <t>bronze</t>
-  </si>
-  <si>
-    <t>sgs</t>
-  </si>
-  <si>
-    <t>samis</t>
-  </si>
-  <si>
-    <t>platinum</t>
-  </si>
-  <si>
-    <t>gold</t>
+    <t>Master</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,13 +432,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -440,15 +446,29 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>